<commit_message>
Change  Name file Round 2 Evaluation Round 3
</commit_message>
<xml_diff>
--- a/.idea/files/Evaluation/Round2/EvaluationDataset2-CEA.xlsx
+++ b/.idea/files/Evaluation/Round2/EvaluationDataset2-CEA.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTHONY\IdeaProjects\STI_Thesis\.idea\files\Evaluation\Round2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTHONY\IdeaProjects\STI_Thesis\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D693E42B-6F5F-4132-BD56-9A722ED877E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A9B822-39D6-4128-8EEC-25FB202F7F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1665" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,7 +29,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="203">
+  <si>
+    <t>File name - column - row - URI</t>
+  </si>
   <si>
     <t>Cel Annoted</t>
   </si>
@@ -43,10 +43,592 @@
     <t>Target Cell</t>
   </si>
   <si>
+    <t>Value Target Annoted</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "0" URI:http://dbpedia.org/resource/Yellowfin_cutthroat_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Yellowfin_Cutthroat_Trout http://dbpedia.org/resource/Oncorhynchus_clarki_macdonaldi http://dbpedia.org/resource/Yellowfin_cutthroat_trout http://dbpedia.org/resource/Salmo_clarki_macdonaldi</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "0" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Salmonids http://dbpedia.org/resource/Salmoniform http://dbpedia.org/resource/Salmonidae http://dbpedia.org/resource/Salmon_and_Salmonidae http://dbpedia.org/resource/Salmonid http://dbpedia.org/resource/Salmoniformes</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "0" URI:http://dbpedia.org/resource/Cutthroat_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Oncorhynchus_clarkii http://dbpedia.org/resource/Wyoming_state_fish http://dbpedia.org/resource/Cutthroat_Trout http://dbpedia.org/resource/Oncorhynchus_clarki http://dbpedia.org/resource/Cutthroat_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "0" URI:http://dbpedia.org/resource/TNC</t>
+  </si>
+  <si>
     <t>nan</t>
   </si>
   <si>
-    <t>File name - column - row - URI</t>
+    <t>ResultatDataset1 "4" "0" URI:http://dbpedia.org/resource/GX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "0" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oncorhynchus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "1" URI:http://dbpedia.org/resource/Tecopa_pupfish</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Tecopa_Pupfish http://dbpedia.org/resource/Tecopa_pupfish http://dbpedia.org/resource/Cyprinodon_nevadensis_calidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "1" URI:http://dbpedia.org/resource/Pupfish</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Cyprinodont http://dbpedia.org/resource/Cyprinodontidae http://dbpedia.org/resource/Pupfish http://dbpedia.org/resource/Cyprinodonts http://dbpedia.org/resource/Cyprinodontid http://dbpedia.org/resource/Cyprinodontoidea</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "1" URI:http://dbpedia.org/resource/Cyprinodon_nevadensis</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Amargosa_pupfish http://dbpedia.org/resource/Cyprinodon_nevadensis</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "1" URI:http://dbpedia.org/resource/9950_ESA</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "1" URI:http://dbpedia.org/resource/EX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "1" URI:Cyprinodon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyprinodon </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "2" URI:http://dbpedia.org/resource/Shoshone_pupfish</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Shoshone_pupfish http://dbpedia.org/resource/Shoshone_Pupfish http://dbpedia.org/resource/Cyprinodon_nevadensis_shoshone</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "2" URI:http://dbpedia.org/resource/Pupfish</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "2" URI:http://dbpedia.org/resource/Cyprinodon_nevadensis</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "2" URI:IUCN2.3</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "2" URI:http://dbpedia.org/resource/EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "2" URI:Cyprinodon </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "3" URI:http://dbpedia.org/resource/Sheepshead_minnow</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Cyprinodon_variegatus_variegatus http://dbpedia.org/resource/Sheepshead_minnow http://dbpedia.org/resource/Cyprinodon_variegatus http://dbpedia.org/resource/Sheepshead_Minnow</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "3" URI:http://dbpedia.org/resource/Pupfish</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "3" URI:http://dbpedia.org/resource/Sheepshead_minnow</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "3" URI:IUCN3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "3" URI:http://dbpedia.org/resource/LC</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "5" "3" URI:nan</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "4" URI:http://dbpedia.org/resource/Sea_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Sea_trout http://dbpedia.org/resource/Salmo_trutta_trutta</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "4" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "4" URI:http://dbpedia.org/resource/Brown_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Salmo_Trutta http://dbpedia.org/resource/S._trutta_lacustris http://dbpedia.org/resource/Sewin http://dbpedia.org/resource/Brown_trout http://dbpedia.org/resource/Brown_Trout http://dbpedia.org/resource/Salmo_trutta_morpha_trutta http://dbpedia.org/resource/Sea_Trout http://dbpedia.org/resource/Salmo_trutta_lacustris http://dbpedia.org/resource/S._trutta_morpha_lacustris http://dbpedia.org/resource/Salmo_trutta_forma_fario http://dbpedia.org/resource/Kumdza http://dbpedia.org/resource/Jayboo http://dbpedia.org/resource/Salmo_trutta</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "4" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "4" URI:http://dbpedia.org/resource/LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "4" URI:Salmo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmo </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "5" URI:http://dbpedia.org/resource/Salmo_trutta_fario</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/River_trout http://dbpedia.org/resource/Salmo_trutta_fario http://dbpedia.org/resource/S._trutta_fario http://dbpedia.org/resource/Salmo_trutta_morpha_fario</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "5" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "5" URI:http://dbpedia.org/resource/Brown_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "5" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "5" URI:http://dbpedia.org/resource/LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "5" URI:Salmo </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "6" URI:http://dbpedia.org/resource/Redfin_pickerel</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Redfin_pickerel http://dbpedia.org/resource/Esox_americanus_americanus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "6" URI:http://dbpedia.org/resource/Esox</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Esocid http://dbpedia.org/resource/Esox_(genus) http://dbpedia.org/resource/Pike_(zoology) http://dbpedia.org/resource/Esox http://dbpedia.org/resource/Lucy_(heraldry) http://dbpedia.org/resource/Pike_(fish) http://dbpedia.org/resource/Esocidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "6" URI:http://dbpedia.org/resource/American_pickerel</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Grass_pickerel http://dbpedia.org/resource/Grass_Pickerel http://dbpedia.org/resource/Esox_americanus_vermiculatus http://dbpedia.org/resource/American_pickerel http://dbpedia.org/resource/Redfin_Pickerel http://dbpedia.org/resource/American_Pickerel http://dbpedia.org/resource/Esox_vermiculatus http://dbpedia.org/resource/Esox_americanus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "6" URI:IUCN3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "6" URI:http://dbpedia.org/resource/LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "6" URI:Esox </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esox </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "7" URI:http://dbpedia.org/resource/Oncorhynchus_masou_formosanus</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Oncorhynchus_formosanus http://dbpedia.org/resource/Formosan_landlocked_salmon http://dbpedia.org/resource/Oncorhynchus_masou_formosanus http://dbpedia.org/resource/Taiwanese_salmon http://dbpedia.org/resource/Formosan_Landlocked_Salmon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "7" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "7" URI:http://dbpedia.org/resource/Oncorhynchus_masou</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Japanese_salmon http://dbpedia.org/resource/Masou http://dbpedia.org/resource/Yamame http://dbpedia.org/resource/Oncorhynchus_masou http://dbpedia.org/resource/Oncorhynchus_masu http://dbpedia.org/resource/Seema_(fish) http://dbpedia.org/resource/Cherry_Salmon http://dbpedia.org/resource/Masu_salmon http://dbpedia.org/resource/Cherry_salmon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "7" URI:IUCN2.3</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "7" URI:http://dbpedia.org/resource/CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "7" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "8" URI:http://dbpedia.org/resource/Montana_Arctic_grayling</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Montana_arctic_grayling http://dbpedia.org/resource/Montana_Arctic_grayling</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "8" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "8" URI:http://dbpedia.org/resource/Arctic_grayling</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Alaska_grayling http://dbpedia.org/resource/Arctic_grayling http://dbpedia.org/resource/Alaska_Grayling http://dbpedia.org/resource/Thymallus_montanus http://dbpedia.org/resource/Thymallus_tricolor http://dbpedia.org/resource/Arctic_Grayling http://dbpedia.org/resource/Thymallus_arcticus_arcticus http://dbpedia.org/resource/Thymallus_arcticus http://dbpedia.org/resource/Thymallus_signifer</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "8" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "8" URI:http://dbpedia.org/resource/LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "8" URI:Thymallus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thymallus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "9" URI:http://dbpedia.org/resource/Mohave_tui_chub</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Mohave_chub http://dbpedia.org/resource/Mojave_tui_chub http://dbpedia.org/resource/Mojave_chub http://dbpedia.org/resource/Gila_bicolor_mohavensis http://dbpedia.org/resource/Mohave_tui_chub http://dbpedia.org/resource/Siphateles_bicolor_mohavensis</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "9" URI:http://dbpedia.org/resource/Cyprinidae</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Mountain_carp http://dbpedia.org/resource/Cyprinoid http://dbpedia.org/resource/Cyprinidae http://dbpedia.org/resource/Cyprinids http://dbpedia.org/resource/Cyprinid http://dbpedia.org/resource/Chub_(zoology)</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "9" URI:http://dbpedia.org/resource/Tui_chub</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Tui_Chub http://dbpedia.org/resource/Hutton_Springs_tui_chub http://dbpedia.org/resource/Tui_chub http://dbpedia.org/resource/Gila_bicolor</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "9" URI:http://dbpedia.org/resource/9950_ESA</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "9" URI:http://dbpedia.org/resource/LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "9" URI:Siphateles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siphateles </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "10" URI:http://dbpedia.org/resource/Little_Kern_golden_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Little_Kern_golden_trout http://dbpedia.org/resource/Little_Kern_Golden_Trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "10" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "10" URI:http://dbpedia.org/resource/Rainbow_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Steelhead_(fish) http://dbpedia.org/resource/Salmo_gairdneri http://dbpedia.org/resource/Golden_Rainbow_Trout http://dbpedia.org/resource/Parasalmo_mykiss http://dbpedia.org/resource/Raibow_Trout http://dbpedia.org/resource/Coastal_rainbow_trout http://dbpedia.org/resource/Oncorhyncus_mykiss http://dbpedia.org/resource/Rainbow_Trout http://dbpedia.org/resource/Steelhead_trout http://dbpedia.org/resource/Steelhead_salmon http://dbpedia.org/resource/Salmon_trout http://dbpedia.org/resource/Rainbow_trout http://dbpedia.org/resource/Onchorhynchus_mykiss http://dbpedia.org/resource/Steelhead_Trout http://dbpedia.org/resource/Oncorhynchus_mykiss http://dbpedia.org/resource/Salmo_iridia http://dbpedia.org/resource/Steelhead http://dbpedia.org/resource/Nijimasu_no_shioyaki http://dbpedia.org/resource/Ocean_trout http://dbpedia.org/resource/Mykiss http://dbpedia.org/resource/Splck</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "10" URI:http://dbpedia.org/resource/9950_ESA</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "10" URI:http://dbpedia.org/resource/LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "10" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "11" URI:http://dbpedia.org/resource/Kirikuchi_char</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Kirikuchi_char http://dbpedia.org/resource/Salvelinus_japonicus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "11" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "11" URI:http://dbpedia.org/resource/Salvelinus_leucomaenis</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Whitespotted_char http://dbpedia.org/resource/Salvelinus_leucomaenis http://dbpedia.org/resource/White-spotted_char</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "11" URI:IUCN2.3</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "11" URI:http://dbpedia.org/resource/EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "11" URI:Salvelinus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvelinus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "12" URI:http://dbpedia.org/resource/Independence_Valley_tui_chub</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Siphateles_bicolor_isolata http://dbpedia.org/resource/Independence_Valley_Tui_Chub http://dbpedia.org/resource/Gila_bicolor_isolata http://dbpedia.org/resource/Independence_Valley_tui_chub</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "12" URI:http://dbpedia.org/resource/Cyprinidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "12" URI:http://dbpedia.org/resource/Tui_chub</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "12" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "12" URI:http://dbpedia.org/resource/EX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "12" URI:Siphateles </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "13" URI:http://dbpedia.org/resource/Gulf_sturgeon</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Acipenser_oxyrinchus_desotoi http://dbpedia.org/resource/Acipenser_oxyrhynchus_desotoi http://dbpedia.org/resource/Gulf_Sturgeon http://dbpedia.org/resource/Gulf_sturgeon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "13" URI:http://dbpedia.org/resource/Sturgeon</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Sturgeons http://dbpedia.org/resource/True_Sturgeon http://dbpedia.org/resource/Acipenserid http://dbpedia.org/resource/Acipenseridae http://dbpedia.org/resource/Acipenser_Endangered http://dbpedia.org/resource/Acipenserids http://dbpedia.org/resource/Threatened_sturgeons http://dbpedia.org/resource/Accipenser http://dbpedia.org/resource/Albany_beef http://dbpedia.org/resource/True_Sturgeons http://dbpedia.org/resource/Sturgeon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "13" URI:http://dbpedia.org/resource/Acipenser_oxyrinchus</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Acipenser_oxyrinchus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "13" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "13" URI:http://dbpedia.org/resource/VU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "13" URI:Acipenser </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acipenser </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "14" URI:http://dbpedia.org/resource/Greenback_cutthroat_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Oncorhynchus_clarki_stomias http://dbpedia.org/resource/Colorado_state_fish http://dbpedia.org/resource/Oncorhynchus_clarkii_stomias http://dbpedia.org/resource/Greenback_Cutthroat_Trout http://dbpedia.org/resource/Greenback_cutthroat_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "14" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "14" URI:http://dbpedia.org/resource/Cutthroat_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "14" URI:http://dbpedia.org/resource/9950_ESA</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "14" URI:http://dbpedia.org/resource/T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "14" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "15" URI:http://dbpedia.org/resource/Golden_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Golden_trout http://dbpedia.org/resource/California_golden_trout http://dbpedia.org/resource/Golden_Trout http://dbpedia.org/resource/Oncorhynchus_aguabonita http://dbpedia.org/resource/Oncorhynchus_mykiss_aguabonita</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "15" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "15" URI:http://dbpedia.org/resource/Rainbow_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "15" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "15" URI:http://dbpedia.org/resource/NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "15" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "16" URI:http://dbpedia.org/resource/Dead_Sea_toothcarp</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Dead_Sea_toothcarp http://dbpedia.org/resource/Aphanius_dispar_richardsoni</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "16" URI:http://dbpedia.org/resource/Pupfish</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "16" URI:http://dbpedia.org/resource/Arabian_toothcarp</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Cyprinodon_cilensis http://dbpedia.org/resource/Cyprinodon_hammonis http://dbpedia.org/resource/Cyprinodon_moseas http://dbpedia.org/resource/Lebias_dispar http://dbpedia.org/resource/Cyprinodon_richardsoni http://dbpedia.org/resource/Lebias_velifer http://dbpedia.org/resource/Aphanius_dispar_dispar http://dbpedia.org/resource/Cyprinodon_lunatus http://dbpedia.org/resource/Arabian_toothcarp http://dbpedia.org/resource/Lebias_lunatus http://dbpedia.org/resource/Aphanius_dispar http://dbpedia.org/resource/Cyprinodon_stoliczkanus http://dbpedia.org/resource/Cyprinodon_darrorensis</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "16" URI:IUCN3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "16" URI:http://dbpedia.org/resource/EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "16" URI:Aphanius </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aphanius </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "17" URI:http://dbpedia.org/resource/Catostomus_discobolus_jarrovii</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Zuni_bluehead_Sucker http://dbpedia.org/resource/Catostomus_discobolus_jarrovii http://dbpedia.org/resource/Zuni_Bluehead_Sucker http://dbpedia.org/resource/Zuni_bluehead_sucker http://dbpedia.org/resource/Zuni_Bluehead_sucker http://dbpedia.org/resource/Catostomus_discobolus_yarrowi</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "17" URI:http://dbpedia.org/resource/Catostomidae</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Catostomid http://dbpedia.org/resource/Catostomidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "17" URI:http://dbpedia.org/resource/Catostomus_discobolus</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Catostomus_discobolus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "17" URI:IUCN2.3</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "17" URI:http://dbpedia.org/resource/VU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "17" URI:Catostomus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catostomus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "18" URI:http://dbpedia.org/resource/Catostomus_catostomus_cristatus</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Catostomus_catostomus_cristatus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "18" URI:http://dbpedia.org/resource/Catostomidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "18" URI:http://dbpedia.org/resource/Longnose_sucker</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Longnose_sucker http://dbpedia.org/resource/Catostomus_catostomus http://dbpedia.org/resource/Catostomus_catostomus_catostomus http://dbpedia.org/resource/Longnose_Sucker http://dbpedia.org/resource/Common_northern_sucker</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "18" URI:IUCN2.3</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "18" URI:http://dbpedia.org/resource/EX</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "5" "18" URI:nan</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "19" URI:http://dbpedia.org/resource/Baikal_sturgeon</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/A._baerii_baicalensis http://dbpedia.org/resource/Acipenser_baerii_baikalensis http://dbpedia.org/resource/Acipenser_baerii_baicalensis http://dbpedia.org/resource/Baikal_Sturgeon http://dbpedia.org/resource/Baikal_sturgeon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "19" URI:http://dbpedia.org/resource/Sturgeon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "19" URI:http://dbpedia.org/resource/Siberian_sturgeon</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Acipenser_baerii http://dbpedia.org/resource/Acipenser_baerii_baerii http://dbpedia.org/resource/Siberian_sturgeon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "19" URI:iucn2.3</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "19" URI:http://dbpedia.org/resource/EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "19" URI:Acipenser </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "20" URI:http://dbpedia.org/resource/Atlantic_sturgeon</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Atlantic_Sturgeon http://dbpedia.org/resource/Acipenser_oxyrinchus_oxyrinchus http://dbpedia.org/resource/Acipenser_oxyrhinchus http://dbpedia.org/resource/Atlantic_sturgeon http://dbpedia.org/resource/Acipenser_oxyrhynchus_oxyrhynchus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "20" URI:http://dbpedia.org/resource/Sturgeon</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "20" URI:http://dbpedia.org/resource/Acipenser_oxyrinchus</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "20" URI:IUCN3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "20" URI:http://dbpedia.org/resource/NT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "20" URI:Acipenser </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "21" URI:http://dbpedia.org/resource/Athabasca_rainbow_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Athabasca_rainbow_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "21" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "21" URI:http://dbpedia.org/resource/Rainbow_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "21" URI:iucn3.1</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "21" URI:http://dbpedia.org/resource/NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "21" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "0" "22" URI:http://dbpedia.org/resource/Alvord_cutthroat_trout</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Oncorhynchus_clarki_alvordensis http://dbpedia.org/resource/Alvord_cutthroat_trout http://dbpedia.org/resource/Alvord_Cutthroat_Trout http://dbpedia.org/resource/Alvord_cutthroat</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "1" "22" URI:http://dbpedia.org/resource/Salmonidae</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "2" "22" URI:http://dbpedia.org/resource/Cutthroat_trout</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "3" "22" URI:http://dbpedia.org/resource/TNC</t>
+  </si>
+  <si>
+    <t>ResultatDataset1 "4" "22" URI:http://dbpedia.org/resource/GX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResultatDataset1 "5" "22" URI:Oncorhynchus </t>
+  </si>
+  <si>
+    <t>Cell Not Added</t>
+  </si>
+  <si>
+    <t>Cell Added</t>
+  </si>
+  <si>
+    <t>Cell Not added</t>
   </si>
   <si>
     <t xml:space="preserve">Précision </t>
@@ -55,518 +637,25 @@
     <t xml:space="preserve">Recall </t>
   </si>
   <si>
-    <t>Value Target Annoted</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "1" URI: http://dbpedia.org/resource/Yellowfin_cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "1" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "1" URI: http://dbpedia.org/resource/Cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "1" URI: http://dbpedia.org/resource/TNC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "1" URI: http://dbpedia.org/resource/GX</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "3" URI: http://dbpedia.org/resource/9950_ESA</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "4" URI: http://dbpedia.org/resource/Pupfish</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "4" URI: http://dbpedia.org/resource/Cyprinodon_nevadensis</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "5" URI: http://dbpedia.org/resource/Pupfish</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "6" URI: http://dbpedia.org/resource/LC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "7" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "7" URI: http://dbpedia.org/resource/Brown_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "7" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "7" URI: http://dbpedia.org/resource/LC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "8" URI: http://dbpedia.org/resource/LC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "10" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "11" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "12" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "14" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "16" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Yellowfin_Cutthroat_Trout http://dbpedia.org/resource/Oncorhynchus_clarki_macdonaldi http://dbpedia.org/resource/Yellowfin_cutthroat_trout http://dbpedia.org/resource/Salmo_clarki_macdonaldihttp://dbpedia.org/resource/Westminster_College_(Fulton,_MO) http://dbpedia.org/resource/Westminster_College,_Missouri</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Salmonids http://dbpedia.org/resource/Salmoniform http://dbpedia.org/resource/Salmonidae http://dbpedia.org/resource/Salmon_and_Salmonidae http://dbpedia.org/resource/Salmonid http://dbpedia.org/resource/Salmoniformes</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Oncorhynchus_clarkii http://dbpedia.org/resource/Wyoming_state_fish http://dbpedia.org/resource/Cutthroat_Trout http://dbpedia.org/resource/Oncorhynchus_clarki http://dbpedia.org/resource/Cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "2" URI: http://dbpedia.org/resource/9950_ESA</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "3" URI: http://dbpedia.org/resource/Pupfish</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "3" URI: http://dbpedia.org/resource/Cyprinodon_nevadensis</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "5" URI: http://dbpedia.org/resource/LC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "6" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "6" URI: http://dbpedia.org/resource/Brown_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "6" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "9" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "11" URI: http://dbpedia.org/resource/Little_Kern_golden_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "11" URI: http://dbpedia.org/resource/Rainbow_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "11" URI: http://dbpedia.org/resource/9950_ESA</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "11" URI: http://dbpedia.org/resource/LT</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "12" URI: http://dbpedia.org/resource/Kirikuchi_char</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "12" URI: http://dbpedia.org/resource/Salvelinus_leucomaenis</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "12" URI: IUCN2.3</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "12" URI: http://dbpedia.org/resource/EN</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "13" URI: http://dbpedia.org/resource/Independence_Valley_tui_chub</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "13" URI: http://dbpedia.org/resource/Cyprinidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "13" URI: http://dbpedia.org/resource/Tui_chub</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "13" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "13" URI: http://dbpedia.org/resource/EX</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "14" URI: http://dbpedia.org/resource/Gulf_sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "14" URI: http://dbpedia.org/resource/Sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "14" URI: http://dbpedia.org/resource/Acipenser_oxyrinchus</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "14" URI: http://dbpedia.org/resource/VU</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "15" URI: http://dbpedia.org/resource/Greenback_cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "15" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "15" URI: http://dbpedia.org/resource/Cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "15" URI: http://dbpedia.org/resource/9950_ESA</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "15" URI: http://dbpedia.org/resource/T</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "16" URI: http://dbpedia.org/resource/Golden_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "16" URI: http://dbpedia.org/resource/Rainbow_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "16" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "16" URI: http://dbpedia.org/resource/NE</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "17" URI: http://dbpedia.org/resource/Dead_Sea_toothcarp</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "17" URI: http://dbpedia.org/resource/Pupfish</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "17" URI: http://dbpedia.org/resource/Arabian_toothcarp</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "17" URI: IUCN3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "17" URI: http://dbpedia.org/resource/EN</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "18" URI: http://dbpedia.org/resource/Catostomus_discobolus_jarrovii</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Sea_trout http://dbpedia.org/resource/Salmo_trutta_trutta</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/River_trout http://dbpedia.org/resource/Salmo_trutta_fario http://dbpedia.org/resource/S._trutta_fario http://dbpedia.org/resource/Salmo_trutta_morpha_fario</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Mountain_carp http://dbpedia.org/resource/Cyprinoid http://dbpedia.org/resource/Cyprinidae http://dbpedia.org/resource/Cyprinids http://dbpedia.org/resource/Cyprinid http://dbpedia.org/resource/Chub_(zoology)</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Tui_Chub http://dbpedia.org/resource/Hutton_Springs_tui_chub http://dbpedia.org/resource/Tui_chub http://dbpedia.org/resource/Gila_bicolor</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Little_Kern_golden_trout http://dbpedia.org/resource/Little_Kern_Golden_Trout</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Steelhead_(fish) http://dbpedia.org/resource/Salmo_gairdneri http://dbpedia.org/resource/Golden_Rainbow_Trout http://dbpedia.org/resource/Parasalmo_mykiss http://dbpedia.org/resource/Raibow_Trout http://dbpedia.org/resource/Coastal_rainbow_trout http://dbpedia.org/resource/Oncorhyncus_mykiss http://dbpedia.org/resource/Rainbow_Trout http://dbpedia.org/resource/Steelhead_trout http://dbpedia.org/resource/Steelhead_salmon http://dbpedia.org/resource/Salmon_trout http://dbpedia.org/resource/Rainbow_trout http://dbpedia.org/resource/Onchorhynchus_mykiss http://dbpedia.org/resource/Steelhead_Trout http://dbpedia.org/resource/Oncorhynchus_mykiss http://dbpedia.org/resource/Salmo_iridia http://dbpedia.org/resource/Steelhead http://dbpedia.org/resource/Nijimasu_no_shioyaki http://dbpedia.org/resource/Ocean_trout http://dbpedia.org/resource/Mykiss http://dbpedia.org/resource/Splck</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "18" URI: http://dbpedia.org/resource/Catostomidae</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Zuni_bluehead_Sucker http://dbpedia.org/resource/Catostomus_discobolus_jarrovii http://dbpedia.org/resource/Zuni_Bluehead_Sucker http://dbpedia.org/resource/Zuni_bluehead_sucker http://dbpedia.org/resource/Zuni_Bluehead_sucker http://dbpedia.org/resource/Catostomus_discobolus_yarrowi"</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "22" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "22" URI: http://dbpedia.org/resource/Rainbow_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "22" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "22" URI: http://dbpedia.org/resource/NE</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "2" URI: http://dbpedia.org/resource/Mohave_tui_chub</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "2" URI: http://dbpedia.org/resource/Cyprinidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "2" URI: http://dbpedia.org/resource/Tui_chub</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "2" URI: http://dbpedia.org/resource/LE</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "3" URI: http://dbpedia.org/resource/Tecopa_pupfish</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "3" URI: http://dbpedia.org/resource/EX</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "4" URI: http://dbpedia.org/resource/Shoshone_pupfish</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "4" URI: IUCN2.3</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "4" URI: http://dbpedia.org/resource/EN</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "5" URI: http://dbpedia.org/resource/Sheepshead_minnow</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "5" URI: http://dbpedia.org/resource/Sheepshead_minnow</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "5" URI: IUCN3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "6" URI: http://dbpedia.org/resource/Sea_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "7" URI: http://dbpedia.org/resource/Salmo_trutta_fario</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "8" URI: http://dbpedia.org/resource/Redfin_pickerel</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "8" URI: http://dbpedia.org/resource/Esox</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "8" URI: http://dbpedia.org/resource/American_pickerel</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "8" URI: IUCN3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "9" URI: http://dbpedia.org/resource/Oncorhynchus_masou_formosanus</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "9" URI: http://dbpedia.org/resource/Oncorhynchus_masou</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "9" URI: IUCN2.3</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "9" URI: http://dbpedia.org/resource/CR</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "10" URI: http://dbpedia.org/resource/Montana_Arctic_grayling</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "10" URI: http://dbpedia.org/resource/Arctic_grayling</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "10" URI: iucn3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "10" URI: http://dbpedia.org/resource/LC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "18" URI: http://dbpedia.org/resource/Catostomus_discobolus</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "18" URI: IUCN2.3</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "18" URI: http://dbpedia.org/resource/VU</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "19" URI: http://dbpedia.org/resource/Catostomus_catostomus_cristatus</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "19" URI: http://dbpedia.org/resource/Catostomidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "19" URI: http://dbpedia.org/resource/Longnose_sucker</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "19" URI: IUCN2.3</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "19" URI: http://dbpedia.org/resource/EX</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "20" URI: http://dbpedia.org/resource/Baikal_sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "20" URI: http://dbpedia.org/resource/Sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "20" URI: http://dbpedia.org/resource/Siberian_sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "20" URI: iucn2.3</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "20" URI: http://dbpedia.org/resource/EN</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "21" URI: http://dbpedia.org/resource/Atlantic_sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "21" URI: http://dbpedia.org/resource/Sturgeon</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "21" URI: http://dbpedia.org/resource/Acipenser_oxyrinchus</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "21" URI: IUCN3.1</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "21" URI: http://dbpedia.org/resource/NT</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "22" URI: http://dbpedia.org/resource/Athabasca_rainbow_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "0" "23" URI: http://dbpedia.org/resource/Alvord_cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "1" "23" URI: http://dbpedia.org/resource/Salmonidae</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "2" "23" URI: http://dbpedia.org/resource/Cutthroat_trout</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "3" "23" URI: http://dbpedia.org/resource/TNC</t>
-  </si>
-  <si>
-    <t>ResultatDataset2 "4" "23" URI: http://dbpedia.org/resource/GX</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Acipenser_oxyrinchus</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Mohave_chub http://dbpedia.org/resource/Mojave_tui_chub http://dbpedia.org/resource/Mojave_chub http://dbpedia.org/resource/Gila_bicolor_mohavensis http://dbpedia.org/resource/Mohave_tui_chub http://dbpedia.org/resource/Siphateles_bicolor_mohavensis"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Mountain_carp http://dbpedia.org/resource/Cyprinoid http://dbpedia.org/resource/Cyprinidae http://dbpedia.org/resource/Cyprinids http://dbpedia.org/resource/Cyprinid http://dbpedia.org/resource/Chub_(zoology)"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Tui_Chub http://dbpedia.org/resource/Hutton_Springs_tui_chub http://dbpedia.org/resource/Tui_chub http://dbpedia.org/resource/Gila_bicolor"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Tecopa_Pupfish http://dbpedia.org/resource/Tecopa_pupfish http://dbpedia.org/resource/Cyprinodon_nevadensis_calidae"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Cyprinodont http://dbpedia.org/resource/Cyprinodontidae http://dbpedia.org/resource/Pupfish http://dbpedia.org/resource/Cyprinodonts http://dbpedia.org/resource/Cyprinodontid http://dbpedia.org/resource/Cyprinodontoidea"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Amargosa_pupfish http://dbpedia.org/resource/Cyprinodon_nevadensis"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Shoshone_pupfish http://dbpedia.org/resource/Shoshone_Pupfish http://dbpedia.org/resource/Cyprinodon_nevadensis_shoshone"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Cyprinodon_variegatus_variegatus http://dbpedia.org/resource/Sheepshead_minnow http://dbpedia.org/resource/Cyprinodon_variegatus http://dbpedia.org/resource/Sheepshead_Minnow"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Salmonids http://dbpedia.org/resource/Salmoniform http://dbpedia.org/resource/Salmonidae http://dbpedia.org/resource/Salmon_and_Salmonidae http://dbpedia.org/resource/Salmonid http://dbpedia.org/resource/Salmoniformes"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Salmo_Trutta http://dbpedia.org/resource/S._trutta_lacustris http://dbpedia.org/resource/Sewin http://dbpedia.org/resource/Brown_trout http://dbpedia.org/resource/Brown_Trout http://dbpedia.org/resource/Salmo_trutta_morpha_trutta http://dbpedia.org/resource/Sea_Trout http://dbpedia.org/resource/Salmo_trutta_lacustris http://dbpedia.org/resource/S._trutta_morpha_lacustris http://dbpedia.org/resource/Salmo_trutta_forma_fario http://dbpedia.org/resource/Kumdza http://dbpedia.org/resource/Jayboo http://dbpedia.org/resource/Salmo_trutta"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Esocid http://dbpedia.org/resource/Esox_(genus) http://dbpedia.org/resource/Pike_(zoology) http://dbpedia.org/resource/Esox http://dbpedia.org/resource/Lucy_(heraldry) http://dbpedia.org/resource/Pike_(fish) http://dbpedia.org/resource/Esocidae"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Grass_pickerel http://dbpedia.org/resource/Grass_Pickerel http://dbpedia.org/resource/Esox_americanus_vermiculatus http://dbpedia.org/resource/American_pickerel http://dbpedia.org/resource/Redfin_Pickerel http://dbpedia.org/resource/American_Pickerel http://dbpedia.org/resource/Esox_vermiculatus http://dbpedia.org/resource/Esox_americanus"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Oncorhynchus_formosanus http://dbpedia.org/resource/Formosan_landlocked_salmon http://dbpedia.org/resource/Oncorhynchus_masou_formosanus http://dbpedia.org/resource/Taiwanese_salmon http://dbpedia.org/resource/Formosan_Landlocked_Salmon"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Japanese_salmon http://dbpedia.org/resource/Masou http://dbpedia.org/resource/Yamame http://dbpedia.org/resource/Oncorhynchus_masou http://dbpedia.org/resource/Oncorhynchus_masu http://dbpedia.org/resource/Seema_(fish) http://dbpedia.org/resource/Cherry_Salmon http://dbpedia.org/resource/Masu_salmon http://dbpedia.org/resource/Cherry_salmon"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Montana_arctic_grayling http://dbpedia.org/resource/Montana_Arctic_grayling"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Alaska_grayling http://dbpedia.org/resource/Arctic_grayling http://dbpedia.org/resource/Alaska_Grayling http://dbpedia.org/resource/Thymallus_montanus http://dbpedia.org/resource/Thymallus_tricolor http://dbpedia.org/resource/Arctic_Grayling http://dbpedia.org/resource/Thymallus_arcticus_arcticus http://dbpedia.org/resource/Thymallus_arcticus http://dbpedia.org/resource/Thymallus_signifer"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Kirikuchi_char http://dbpedia.org/resource/Salvelinus_japonicus"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Whitespotted_char http://dbpedia.org/resource/Salvelinus_leucomaenis http://dbpedia.org/resource/White-spotted_char"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Siphateles_bicolor_isolata http://dbpedia.org/resource/Independence_Valley_Tui_Chub http://dbpedia.org/resource/Gila_bicolor_isolata http://dbpedia.org/resource/Independence_Valley_tui_chub"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Sturgeons http://dbpedia.org/resource/True_Sturgeon http://dbpedia.org/resource/Acipenserid http://dbpedia.org/resource/Acipenseridae http://dbpedia.org/resource/Acipenser_Endangered http://dbpedia.org/resource/Acipenserids http://dbpedia.org/resource/Threatened_sturgeons http://dbpedia.org/resource/Accipenser http://dbpedia.org/resource/Albany_beef http://dbpedia.org/resource/True_Sturgeons http://dbpedia.org/resource/Sturgeon"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Acipenser_oxyrinchus_desotoi http://dbpedia.org/resource/Acipenser_oxyrhynchus_desotoi http://dbpedia.org/resource/Gulf_Sturgeon http://dbpedia.org/resource/Gulf_sturgeon"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Acipenser_oxyrinchus"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Oncorhynchus_clarki_stomias http://dbpedia.org/resource/Colorado_state_fish http://dbpedia.org/resource/Oncorhynchus_clarkii_stomias http://dbpedia.org/resource/Greenback_Cutthroat_Trout http://dbpedia.org/resource/Greenback_cutthroat_trout"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Oncorhynchus_clarkii http://dbpedia.org/resource/Wyoming_state_fish http://dbpedia.org/resource/Cutthroat_Trout http://dbpedia.org/resource/Oncorhynchus_clarki http://dbpedia.org/resource/Cutthroat_trout"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Little_Kern_golden_trout http://dbpedia.org/resource/Little_Kern_Golden_Trout"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Steelhead_(fish) http://dbpedia.org/resource/Salmo_gairdneri http://dbpedia.org/resource/Golden_Rainbow_Trout http://dbpedia.org/resource/Parasalmo_mykiss http://dbpedia.org/resource/Raibow_Trout http://dbpedia.org/resource/Coastal_rainbow_trout http://dbpedia.org/resource/Oncorhyncus_mykiss http://dbpedia.org/resource/Rainbow_Trout http://dbpedia.org/resource/Steelhead_trout http://dbpedia.org/resource/Steelhead_salmon http://dbpedia.org/resource/Salmon_trout http://dbpedia.org/resource/Rainbow_trout http://dbpedia.org/resource/Onchorhynchus_mykiss http://dbpedia.org/resource/Steelhead_Trout http://dbpedia.org/resource/Oncorhynchus_mykiss http://dbpedia.org/resource/Salmo_iridia http://dbpedia.org/resource/Steelhead http://dbpedia.org/resource/Nijimasu_no_shioyaki http://dbpedia.org/resource/Ocean_trout http://dbpedia.org/resource/Mykiss http://dbpedia.org/resource/Splck"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Dead_Sea_toothcarp http://dbpedia.org/resource/Aphanius_dispar_richardsoni"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Cyprinodon_cilensis http://dbpedia.org/resource/Cyprinodon_hammonis http://dbpedia.org/resource/Cyprinodon_moseas http://dbpedia.org/resource/Lebias_dispar http://dbpedia.org/resource/Cyprinodon_richardsoni http://dbpedia.org/resource/Lebias_velifer http://dbpedia.org/resource/Aphanius_dispar_dispar http://dbpedia.org/resource/Cyprinodon_lunatus http://dbpedia.org/resource/Arabian_toothcarp http://dbpedia.org/resource/Lebias_lunatus http://dbpedia.org/resource/Aphanius_dispar http://dbpedia.org/resource/Cyprinodon_stoliczkanus http://dbpedia.org/resource/Cyprinodon_darrorensis"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Catostomid http://dbpedia.org/resource/Catostomidae"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Catostomus_discobolus"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Catostomus_catostomus_cristatus"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Longnose_sucker http://dbpedia.org/resource/Catostomus_catostomus http://dbpedia.org/resource/Catostomus_catostomus_catostomus http://dbpedia.org/resource/Longnose_Sucker http://dbpedia.org/resource/Common_northern_sucker"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/A._baerii_baicalensis http://dbpedia.org/resource/Acipenser_baerii_baikalensis http://dbpedia.org/resource/Acipenser_baerii_baicalensis http://dbpedia.org/resource/Baikal_Sturgeon http://dbpedia.org/resource/Baikal_sturgeon"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Acipenser_baerii http://dbpedia.org/resource/Acipenser_baerii_baerii http://dbpedia.org/resource/Siberian_sturgeon"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Atlantic_Sturgeon http://dbpedia.org/resource/Acipenser_oxyrinchus_oxyrinchus http://dbpedia.org/resource/Acipenser_oxyrhinchus http://dbpedia.org/resource/Atlantic_sturgeon http://dbpedia.org/resource/Acipenser_oxyrhynchus_oxyrhynchus"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Athabasca_rainbow_trout"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Oncorhynchus_clarki_alvordensis http://dbpedia.org/resource/Alvord_cutthroat_trout http://dbpedia.org/resource/Alvord_Cutthroat_Trout http://dbpedia.org/resource/Alvord_cutthroat"</t>
-  </si>
-  <si>
-    <t>http://dbpedia.org/resource/Redfin_pickerel http://dbpedia.org/resource/Esox_americanus_americanus</t>
-  </si>
-  <si>
-    <t>SemTab Round 2 - 274.csv &amp; 275.csv</t>
-  </si>
-  <si>
-    <t>F1-Score</t>
+    <t>F1_Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -576,9 +665,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -592,7 +681,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -600,24 +689,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -630,7 +735,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -640,44 +745,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -704,32 +809,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -756,24 +843,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -785,199 +854,230 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="J137" sqref="J137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="95" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>172</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
       <c r="E3">
-        <f>IF(D3 = "nan",0,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -992,34 +1092,32 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E67" si="0">IF(D4 = "nan",0,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1028,34 +1126,32 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1064,16 +1160,15 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1082,16 +1177,15 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1100,16 +1194,15 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1118,16 +1211,15 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1136,16 +1228,15 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1154,16 +1245,15 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1172,16 +1262,15 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1190,70 +1279,66 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1262,16 +1347,15 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>25</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1280,88 +1364,83 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1370,52 +1449,49 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1424,88 +1500,83 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1514,16 +1585,15 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1532,34 +1602,32 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>44</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1568,34 +1636,32 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1604,16 +1670,15 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1622,16 +1687,15 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1640,16 +1704,15 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1658,34 +1721,32 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1694,16 +1755,15 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1712,16 +1772,15 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1730,70 +1789,66 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>8</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1802,16 +1857,15 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1820,88 +1874,83 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1910,52 +1959,49 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E55">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1964,88 +2010,83 @@
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="E58">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="E59">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>151</v>
+        <v>12</v>
       </c>
       <c r="E60">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="E62">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2054,16 +2095,15 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>152</v>
+        <v>8</v>
       </c>
       <c r="E63">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2072,70 +2112,66 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E64">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
+        <v>12</v>
       </c>
       <c r="E65">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E66">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E67">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2144,16 +2180,15 @@
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E117" si="1">IF(D68 = "nan",0,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2162,16 +2197,15 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2179,17 +2213,16 @@
       <c r="C70">
         <v>1</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>133</v>
+      <c r="D70" t="s">
+        <v>105</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -2198,34 +2231,32 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2234,16 +2265,15 @@
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2252,16 +2282,15 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2270,70 +2299,66 @@
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="E78">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2342,16 +2367,15 @@
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="E79">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2360,142 +2384,134 @@
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="E80">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="E82">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>160</v>
+        <v>12</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="E85">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>3</v>
+        <v>128</v>
       </c>
       <c r="E86">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E87">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2504,88 +2520,83 @@
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="E88">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="E89">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="B90">
         <v>1</v>
       </c>
       <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>163</v>
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>12</v>
       </c>
       <c r="E90">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E91">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="E92">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2593,17 +2604,16 @@
       <c r="C93">
         <v>1</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>164</v>
+      <c r="D93" t="s">
+        <v>8</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2612,34 +2622,32 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="E94">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="E95">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -2648,34 +2656,32 @@
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E96">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B97">
         <v>1</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E97">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2684,34 +2690,32 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="E99">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2720,16 +2724,15 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="E100">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -2738,34 +2741,32 @@
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E101">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E102">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2774,34 +2775,32 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="E103">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E104">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2809,71 +2808,67 @@
       <c r="C105">
         <v>1</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>155</v>
+      <c r="D105" t="s">
+        <v>153</v>
       </c>
       <c r="E105">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>3</v>
+        <v>155</v>
       </c>
       <c r="E106">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E107">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>1</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>169</v>
+        <v>0</v>
+      </c>
+      <c r="D108" t="s">
+        <v>12</v>
       </c>
       <c r="E108">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2882,106 +2877,100 @@
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="E109">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E110">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="E111">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>3</v>
+        <v>164</v>
       </c>
       <c r="E112">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E113">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="E114">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2990,98 +2979,513 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="E115">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="B116">
         <v>1</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>3</v>
+        <v>169</v>
       </c>
       <c r="E116">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="E117">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>171</v>
+      </c>
       <c r="B118">
-        <f>SUM(B3:B117)</f>
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="C118">
-        <f>SUM(C3:C117)</f>
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="D118" t="s">
+        <v>172</v>
       </c>
       <c r="E118">
-        <f>SUM(E3:E117)</f>
-        <v>69</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>173</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>174</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>5</v>
-      </c>
-      <c r="B121" s="1">
-        <f>C118/B118</f>
-        <v>0.66326530612244894</v>
+        <v>175</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121" t="s">
+        <v>126</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>6</v>
-      </c>
-      <c r="B122" s="1">
-        <f>C118/E118</f>
-        <v>0.94202898550724634</v>
+        <v>176</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122" t="s">
+        <v>177</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>173</v>
-      </c>
-      <c r="B123" s="1">
-        <f>(2*B121*B122)/(B121+B122)</f>
-        <v>0.77844311377245501</v>
+        <v>178</v>
+      </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123" t="s">
+        <v>120</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>179</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>122</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>180</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125" t="s">
+        <v>12</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>181</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>182</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127" t="s">
+        <v>126</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>183</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>184</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>185</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>186</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130" t="s">
+        <v>97</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>187</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>188</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132" t="s">
+        <v>12</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>189</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133" t="s">
+        <v>15</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>190</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134" t="s">
+        <v>191</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>192</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>193</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136" t="s">
+        <v>10</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>194</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137" t="s">
+        <v>12</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>195</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138" t="s">
+        <v>12</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>196</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139" t="s">
+        <v>15</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B140">
+        <v>81</v>
+      </c>
+      <c r="C140">
+        <v>69</v>
+      </c>
+      <c r="E140">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B141">
+        <v>23</v>
+      </c>
+      <c r="C141">
+        <v>23</v>
+      </c>
+      <c r="E141">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>200</v>
+      </c>
+      <c r="B144" s="3">
+        <f>C140/B140</f>
+        <v>0.85185185185185186</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>201</v>
+      </c>
+      <c r="B145" s="3">
+        <f>E140/C140</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>202</v>
+      </c>
+      <c r="B146" s="3">
+        <f>(2*B144*B145)/(B144+B145)</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>200</v>
+      </c>
+      <c r="B149" s="3">
+        <f>C141/B141</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>201</v>
+      </c>
+      <c r="B150" s="3">
+        <f>E141/C141</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>202</v>
+      </c>
+      <c r="B151" s="3">
+        <f>(2*B150*B149)/(B149+B150)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D70" r:id="rId1" xr:uid="{C78DC184-0B7A-45C6-92B6-AB1F998B1AA5}"/>
-    <hyperlink ref="D90" r:id="rId2" xr:uid="{1FB0D1D8-A7BB-46EC-94CB-D479ADC07216}"/>
-    <hyperlink ref="D93" r:id="rId3" xr:uid="{05F81DB7-5353-47ED-9B4A-AF227ABBC157}"/>
-    <hyperlink ref="D105" r:id="rId4" xr:uid="{1FA05062-D1FA-4EBD-96F9-0B07B6119F21}"/>
-    <hyperlink ref="D108" r:id="rId5" xr:uid="{BD52DED5-71DC-4B1B-83BF-55F3A8A70B4C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>